<commit_message>
Add results of framework comparison.
</commit_message>
<xml_diff>
--- a/evaluation/dataset_cmp/dataset_openqasm_qiskit.xlsx
+++ b/evaluation/dataset_cmp/dataset_openqasm_qiskit.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\quantum-pattern-detector\evaluation\dataset_cmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A368D618-1441-4FB0-A868-285A9133E445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E443BD78-AB25-4EB3-B2F9-451D7A49F4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A39B132-7E24-4ACB-870A-1CF1FFE4D1F5}"/>
   </bookViews>
@@ -1663,13 +1663,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F462331D-48CE-41D9-84DE-117E466A249A}">
   <dimension ref="A1:AS81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="76" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="86.44140625" customWidth="1"/>
+    <col min="8" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.3">

</xml_diff>